<commit_message>
auto commit Wed Dec 27 11:31:57 CET 2017
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
-    <sheet name="attacks-mitigations" sheetId="2" r:id="rId2"/>
+    <sheet name="leaked datasets" sheetId="3" r:id="rId2"/>
+    <sheet name="attacks-mitigations" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Benefits</t>
   </si>
@@ -202,6 +203,36 @@
   </si>
   <si>
     <t>Educate users</t>
+  </si>
+  <si>
+    <t>Well understood risks</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t># PWs</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>RockYou</t>
+  </si>
+  <si>
+    <t>32 M</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Xato</t>
+  </si>
+  <si>
+    <t>Dropbox</t>
   </si>
 </sst>
 </file>
@@ -311,12 +342,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,7 +671,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -648,7 +682,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -657,7 +691,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -666,7 +700,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -675,7 +709,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -684,82 +718,89 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -768,9 +809,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -781,18 +874,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
@@ -835,7 +928,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B7" t="s">
@@ -878,7 +971,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
@@ -913,7 +1006,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B16" t="s">
@@ -932,7 +1025,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B18" t="s">

</xml_diff>

<commit_message>
auto commit Sat Dec 30 11:15:02 CET 2017
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>Benefits</t>
   </si>
@@ -214,9 +214,6 @@
     <t># PWs</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Literature</t>
   </si>
   <si>
@@ -229,10 +226,43 @@
     <t>LinkedIn</t>
   </si>
   <si>
-    <t>Xato</t>
-  </si>
-  <si>
     <t>Dropbox</t>
+  </si>
+  <si>
+    <t>MySpace</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>http://breachlevelindex.com/top-data-breaches</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>145 M</t>
+  </si>
+  <si>
+    <t>360 M</t>
+  </si>
+  <si>
+    <t>Adobe</t>
+  </si>
+  <si>
+    <t>Yahoo</t>
+  </si>
+  <si>
+    <t>1 B</t>
+  </si>
+  <si>
+    <t>68 M</t>
+  </si>
+  <si>
+    <t>36 M</t>
+  </si>
+  <si>
+    <t>164 M</t>
   </si>
 </sst>
 </file>
@@ -298,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -326,6 +356,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -342,7 +381,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -361,6 +400,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -809,49 +849,108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
+      <c r="C2">
+        <v>2009</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>2012</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto commit Sat Jan  6 12:19:30 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
     <sheet name="leaked datasets" sheetId="3" r:id="rId2"/>
     <sheet name="attacks-mitigations" sheetId="2" r:id="rId3"/>
+    <sheet name="PWRM Benchmark" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,8 +29,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tobias Seitz</author>
+  </authors>
+  <commentList>
+    <comment ref="C13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Tobias Seitz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+you can add "notes" to accounts
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
   <si>
     <t>Benefits</t>
   </si>
@@ -263,13 +297,130 @@
   </si>
   <si>
     <t>164 M</t>
+  </si>
+  <si>
+    <t>Dashlane</t>
+  </si>
+  <si>
+    <t>LastPass</t>
+  </si>
+  <si>
+    <t>1Password</t>
+  </si>
+  <si>
+    <t>PWRM</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Security Audit</t>
+  </si>
+  <si>
+    <t>Password Generation</t>
+  </si>
+  <si>
+    <t>form-detection</t>
+  </si>
+  <si>
+    <t>autofill passwords</t>
+  </si>
+  <si>
+    <t>autofill personal info</t>
+  </si>
+  <si>
+    <t>autofill payment info</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>✘</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>memorization support</t>
+  </si>
+  <si>
+    <t>password hints</t>
+  </si>
+  <si>
+    <t>grouping / tags / folders</t>
+  </si>
+  <si>
+    <t>default groups</t>
+  </si>
+  <si>
+    <t>cross device synchronization</t>
+  </si>
+  <si>
+    <t>personal info wallet</t>
+  </si>
+  <si>
+    <t>on website</t>
+  </si>
+  <si>
+    <t>context aware (policy constraints)</t>
+  </si>
+  <si>
+    <t>strength feedback</t>
+  </si>
+  <si>
+    <t>overall score</t>
+  </si>
+  <si>
+    <t>Integrations</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>negative feedback on reuse</t>
+  </si>
+  <si>
+    <t>password reset</t>
+  </si>
+  <si>
+    <t>(✓)</t>
+  </si>
+  <si>
+    <t>guidance</t>
+  </si>
+  <si>
+    <t>security alert</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desktop </t>
+  </si>
+  <si>
+    <t>Trust</t>
+  </si>
+  <si>
+    <t>Open Source</t>
+  </si>
+  <si>
+    <t>(✘)</t>
+  </si>
+  <si>
+    <t>auto-update password reset</t>
+  </si>
+  <si>
+    <t>Reuse across categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,6 +451,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -366,7 +535,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,8 +549,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -391,6 +584,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -400,21 +594,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -711,7 +929,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -722,7 +940,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -731,7 +949,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -740,7 +958,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -749,7 +967,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -765,7 +983,7 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -776,7 +994,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -785,7 +1003,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -794,7 +1012,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -803,7 +1021,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -812,14 +1030,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -830,7 +1048,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -851,23 +1069,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1150,4 +1368,492 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Sun Jan  7 17:11:18 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -58,12 +58,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="C23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Tobias Seitz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+only premium can warn about private vs business usage of the same passwrods
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="131">
   <si>
     <t>Benefits</t>
   </si>
@@ -362,15 +385,9 @@
     <t>personal info wallet</t>
   </si>
   <si>
-    <t>on website</t>
-  </si>
-  <si>
     <t>context aware (policy constraints)</t>
   </si>
   <si>
-    <t>strength feedback</t>
-  </si>
-  <si>
     <t>overall score</t>
   </si>
   <si>
@@ -389,9 +406,6 @@
     <t>(✓)</t>
   </si>
   <si>
-    <t>guidance</t>
-  </si>
-  <si>
     <t>security alert</t>
   </si>
   <si>
@@ -413,14 +427,65 @@
     <t>auto-update password reset</t>
   </si>
   <si>
-    <t>Reuse across categories</t>
+    <t>Explanation / Motivation</t>
+  </si>
+  <si>
+    <t>Not a core-feature and distracts from "password management" mental model</t>
+  </si>
+  <si>
+    <t>dito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not a core feature, but possibly in future versions. Essential if you change the password in one group. </t>
+  </si>
+  <si>
+    <t>Would be good, but does interfere if it was a group password.</t>
+  </si>
+  <si>
+    <t>Depends on the definition. We make our users type passwords themselves more often which facilitates the memorization of the passwords.</t>
+  </si>
+  <si>
+    <t>Red= needs to be verified</t>
+  </si>
+  <si>
+    <t>strength feedback (ad hoc / in client)</t>
+  </si>
+  <si>
+    <t>ad hoc guidance</t>
+  </si>
+  <si>
+    <t>warn about reuse across groups</t>
+  </si>
+  <si>
+    <t>ad hoc random password</t>
+  </si>
+  <si>
+    <t>Decoy mechanism will be built into it</t>
+  </si>
+  <si>
+    <t>password audit results will be considered</t>
+  </si>
+  <si>
+    <t>WebExtensions allow the extension to run in mobile browsers too, but compatibilty issues persist for the moment</t>
+  </si>
+  <si>
+    <t>Other PWMs require a premium subscription to auto-share passwords. We can't do that at the moment because we don't have a cloud infrastructure</t>
+  </si>
+  <si>
+    <t>It is not necessary to have a standalone application...</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -469,6 +534,21 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -535,7 +615,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -573,8 +653,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -585,6 +677,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,9 +687,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -615,6 +709,12 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -633,6 +733,12 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,7 +1035,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -940,7 +1046,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -949,7 +1055,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -958,7 +1064,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -967,7 +1073,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -983,7 +1089,7 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -994,7 +1100,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1109,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1012,7 +1118,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1127,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1030,14 +1136,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1048,7 +1154,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1372,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,476 +1490,575 @@
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="H1" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11" t="s">
+      <c r="C3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11" t="s">
+      <c r="C4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11" t="s">
+      <c r="C5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11" t="s">
+      <c r="C6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11" t="s">
+      <c r="C30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F33" s="11" t="s">
+      <c r="C33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Wed Jan 10 10:53:55 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
     <sheet name="leaked datasets" sheetId="3" r:id="rId2"/>
     <sheet name="attacks-mitigations" sheetId="2" r:id="rId3"/>
     <sheet name="PWRM Benchmark" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="139">
   <si>
     <t>Benefits</t>
   </si>
@@ -479,6 +480,30 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Analyzing Leaked Data</t>
+  </si>
+  <si>
+    <t>Usage / Purpose</t>
+  </si>
+  <si>
+    <t>Retrospective analysis, ground truth, training guessing algorithms</t>
+  </si>
+  <si>
+    <t>Strengths</t>
+  </si>
+  <si>
+    <t>Weaknesses</t>
+  </si>
+  <si>
+    <t>Dubious sources, no influence, legitimacy, noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real-world data, unbiased, </t>
   </si>
 </sst>
 </file>
@@ -678,6 +703,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,8 +714,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1035,7 +1060,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1046,7 +1071,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1080,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1064,7 +1089,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1073,7 +1098,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1089,7 +1114,7 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1100,7 +1125,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1134,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1143,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1127,7 +1152,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1136,14 +1161,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1154,7 +1179,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1480,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1491,22 +1516,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>81</v>
       </c>
       <c r="H1" s="8" t="s">
@@ -1522,7 +1547,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1633,13 +1658,13 @@
       <c r="C8" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="D8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>91</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -1700,10 +1725,10 @@
       <c r="C12" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="8" t="s">
@@ -1757,10 +1782,10 @@
       <c r="C15" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -1787,13 +1812,13 @@
       <c r="C18" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="12" t="s">
+      <c r="D18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1805,10 +1830,10 @@
       <c r="C19" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="D19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -1859,10 +1884,10 @@
       <c r="C22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -1877,10 +1902,10 @@
       <c r="C23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="12" t="s">
+      <c r="D23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>91</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -2061,4 +2086,53 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="60" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Mon Jan 15 17:24:00 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="attacks-mitigations" sheetId="2" r:id="rId3"/>
     <sheet name="PWRM Benchmark" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="policy taxonomy" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -44,6 +45,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Tobias Seitz:</t>
         </r>
@@ -52,6 +54,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 you can add "notes" to accounts
@@ -67,6 +70,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Tobias Seitz:</t>
         </r>
@@ -75,6 +79,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 only premium can warn about private vs business usage of the same passwrods
@@ -87,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="154">
   <si>
     <t>Benefits</t>
   </si>
@@ -504,6 +509,51 @@
   </si>
   <si>
     <t xml:space="preserve">real-world data, unbiased, </t>
+  </si>
+  <si>
+    <t>comp8</t>
+  </si>
+  <si>
+    <t>2word16</t>
+  </si>
+  <si>
+    <t>3class12</t>
+  </si>
+  <si>
+    <t>basic8 (1class8)</t>
+  </si>
+  <si>
+    <t>Example passwords</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>be at least 16 characters long and include at least two letter sequences that are separated by a non-letter sequence.</t>
+  </si>
+  <si>
+    <t>The password needs to ...</t>
+  </si>
+  <si>
+    <t>be at least 12 characters long and include three different character classes (upper, lower, digits, symbol)</t>
+  </si>
+  <si>
+    <t>be at least 8 characters long</t>
+  </si>
+  <si>
+    <t>bet at least 8 characters long, include at least one character from each character class, and not include a dictionary word</t>
+  </si>
+  <si>
+    <t>password -- monkey123 -- qwerasdf</t>
+  </si>
+  <si>
+    <t>P@ssw0rd -- !M0nkey1 -- LGtjj{Rd;w1u\</t>
+  </si>
+  <si>
+    <t>Password1234 -- 2MonkeysBite -- NfJidl2kdils</t>
+  </si>
+  <si>
+    <t>password.unlocks -- 1-Monkey-Bites -- qwer.asdf.zxcvb.1234</t>
   </si>
 </sst>
 </file>
@@ -553,12 +603,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -691,7 +743,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -714,6 +766,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2092,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2135,4 +2188,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Fri Mar  2 16:20:39 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-6380" yWindow="-23540" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="PWRM Benchmark" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
     <sheet name="policy taxonomy" sheetId="6" r:id="rId6"/>
+    <sheet name="Personality Overview" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +38,7 @@
     <author>Tobias Seitz</author>
   </authors>
   <commentList>
-    <comment ref="C13" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C23" authorId="0">
+    <comment ref="C23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
   <si>
     <t>Benefits</t>
   </si>
@@ -554,13 +555,133 @@
   </si>
   <si>
     <t>password.unlocks -- 1-Monkey-Bites -- qwer.asdf.zxcvb.1234</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Openness</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Conscientiousness</t>
+  </si>
+  <si>
+    <t>Extraversion</t>
+  </si>
+  <si>
+    <t>Agreeableness</t>
+  </si>
+  <si>
+    <t>Neuroticism</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>IT Background</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Difficulty to create 2word12 PW</t>
+  </si>
+  <si>
+    <t>Difficulty to create 1emoji12 PW</t>
+  </si>
+  <si>
+    <t>Attitude</t>
+  </si>
+  <si>
+    <t>Preference of 3class12 policy</t>
+  </si>
+  <si>
+    <t>Preference of 1emoji12 policy</t>
+  </si>
+  <si>
+    <t>Preference of 2word12 policy</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>Length of created PW</t>
+  </si>
+  <si>
+    <t>Time to create PW</t>
+  </si>
+  <si>
+    <t>Overall tendency to judge PW strength</t>
+  </si>
+  <si>
+    <t>Comparing PW strength based on length</t>
+  </si>
+  <si>
+    <t>natural direction, i.e. length (++) means positively associated with longer passwords.</t>
+  </si>
+  <si>
+    <t>Guess number of created PW</t>
+  </si>
+  <si>
+    <t>zxcvbn score of created PW</t>
+  </si>
+  <si>
+    <t>cope by memorizing PW</t>
+  </si>
+  <si>
+    <t>cope by reusing PW</t>
+  </si>
+  <si>
+    <t>cope by using PWM</t>
+  </si>
+  <si>
+    <t>cope by using paper / files</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>ppp</t>
+  </si>
+  <si>
+    <t>pppp</t>
+  </si>
+  <si>
+    <t>Comparing PW strength based on number of classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Comparing PW strength based on digits</t>
+  </si>
+  <si>
+    <t>Comparing PW strength based on uppercase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -627,6 +748,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto Medium"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -654,7 +786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -688,6 +820,15 @@
       <top/>
       <bottom style="double">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,7 +884,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -757,6 +898,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,7 +908,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -819,11 +963,242 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00BFC4"/>
+      <color rgb="FF00C08B"/>
+      <color rgb="FF00BA38"/>
+      <color rgb="FF7CAE00"/>
+      <color rgb="FFDE8C00"/>
+      <color rgb="FFF8766D"/>
+      <color rgb="FFFA81E9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1113,7 +1488,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1124,7 +1499,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1508,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1517,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1526,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1167,7 +1542,7 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1178,7 +1553,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1187,7 +1562,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1571,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1580,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1214,14 +1589,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1232,7 +1607,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -2194,7 +2569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
@@ -2217,7 +2592,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B2" t="s">
@@ -2228,7 +2603,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B3" t="s">
@@ -2239,7 +2614,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B4" t="s">
@@ -2250,7 +2625,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B5" t="s">
@@ -2263,4 +2638,512 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="15">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="15">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="15">
+        <v>3</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="15">
+        <v>3</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:K19">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"nn"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"pp"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"ppp"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"pppp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Sat Mar  3 09:44:45 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -20,7 +20,7 @@
     <sheet name="policy taxonomy" sheetId="6" r:id="rId6"/>
     <sheet name="Personality Overview" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
   <si>
     <t>Benefits</t>
   </si>
@@ -560,24 +560,9 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>Openness</t>
-  </si>
-  <si>
     <t>Study</t>
   </si>
   <si>
-    <t>Conscientiousness</t>
-  </si>
-  <si>
-    <t>Extraversion</t>
-  </si>
-  <si>
-    <t>Agreeableness</t>
-  </si>
-  <si>
-    <t>Neuroticism</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -675,13 +660,64 @@
   </si>
   <si>
     <t>Comparing PW strength based on uppercase</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Number of significant associations (p &lt; 0.05)</t>
+  </si>
+  <si>
+    <t>↗️(&lt; .1)</t>
+  </si>
+  <si>
+    <t>↗️(&lt; .05)</t>
+  </si>
+  <si>
+    <t>↗️(&lt; .01)</t>
+  </si>
+  <si>
+    <t>↗️(&lt; .001)</t>
+  </si>
+  <si>
+    <t>↘️(&lt; .1)</t>
+  </si>
+  <si>
+    <t>↘️(&lt; .05)</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Comparing PWs based on number of classes</t>
+  </si>
+  <si>
+    <t>Comparing PWs based on digits</t>
+  </si>
+  <si>
+    <t>Comparing PWs based on uppercase</t>
+  </si>
+  <si>
+    <t>Comparing PWs based on length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -749,6 +785,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Roboto"/>
@@ -756,11 +798,11 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Roboto Medium"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,8 +827,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF619CFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -830,6 +878,68 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -884,7 +994,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -908,9 +1018,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -963,7 +1086,48 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -980,6 +1144,36 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00BA38"/>
         </patternFill>
       </fill>
@@ -1017,6 +1211,17 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -1027,6 +1232,96 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <color theme="0"/>
       </font>
@@ -1038,6 +1333,17 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -1073,6 +1379,311 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BFC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00C08B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00BA38"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7CAE00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDE8C00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8766D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1184,6 +1795,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF619CFF"/>
       <color rgb="FF00BFC4"/>
       <color rgb="FF00C08B"/>
       <color rgb="FF00BA38"/>
@@ -2642,24 +3254,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
+    <col min="4" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -2667,480 +3273,1020 @@
         <v>154</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>187</v>
+        <v>179</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C4" s="15">
         <v>1</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="H4" s="15"/>
+        <v>182</v>
+      </c>
+      <c r="H4" s="22"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C5" s="15">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C6" s="15">
         <v>1</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>181</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
-        <v>184</v>
+      <c r="H7" s="23" t="s">
+        <v>179</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C8" s="15">
         <v>2</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>187</v>
+      <c r="D8" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C9" s="15">
         <v>2</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C10" s="15">
         <v>2</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>187</v>
+      <c r="D10" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C11" s="15">
         <v>2</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C12" s="16">
         <v>2</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>185</v>
+      <c r="D12" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="16" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C13" s="15">
         <v>3</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="15" t="s">
-        <v>185</v>
+      <c r="H13" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C15" s="15">
         <v>3</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="15" t="s">
-        <v>186</v>
+      <c r="H15" s="22" t="s">
+        <v>181</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C16" s="15">
         <v>3</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="H16" s="15"/>
+        <v>179</v>
+      </c>
+      <c r="H16" s="22"/>
       <c r="I16" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C17" s="15">
         <v>3</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="H17" s="15"/>
+        <v>179</v>
+      </c>
+      <c r="H17" s="22"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C18" s="15">
         <v>3</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>187</v>
+      <c r="D18" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="24">
         <v>3</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6">
+        <v>4</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6">
+        <v>2</v>
+      </c>
+      <c r="H20" s="6">
+        <v>2</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
+        <v>2</v>
+      </c>
+      <c r="K20" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="H33" s="22"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="15">
+        <v>1</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="15">
+        <v>1</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="16">
+        <v>1</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" s="15">
+        <v>2</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" s="15">
+        <v>2</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="15">
+        <v>2</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="15">
+        <v>2</v>
+      </c>
+      <c r="D40" s="19"/>
+      <c r="E40" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="16">
+        <v>2</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="15">
+        <v>3</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="15">
+        <v>3</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="15">
+        <v>3</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="15">
+        <v>3</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="15">
+        <v>3</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
         <v>177</v>
       </c>
+      <c r="B47" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="15">
+        <v>3</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="24">
+        <v>3</v>
+      </c>
+      <c r="D48" s="25"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G48" s="24"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="6">
+        <v>4</v>
+      </c>
+      <c r="E49" s="6">
+        <v>4</v>
+      </c>
+      <c r="F49" s="6">
+        <v>3</v>
+      </c>
+      <c r="G49" s="6">
+        <v>2</v>
+      </c>
+      <c r="H49" s="6">
+        <v>2</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0</v>
+      </c>
+      <c r="J49" s="6">
+        <v>2</v>
+      </c>
+      <c r="K49" s="6">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A49:C49"/>
+  </mergeCells>
   <conditionalFormatting sqref="D2:K19">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>"nn"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>"pp"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"ppp"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"pppp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:K48">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>$E$39</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>$E$38</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>$D$41</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>$E$40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+      <formula>$E$45</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>$D$37</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
auto commit Sat Mar  3 12:35:17 CET 2018
</commit_message>
<xml_diff>
--- a/raw/tables/simple-tables.xlsx
+++ b/raw/tables/simple-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6380" yWindow="-23540" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="38400" windowHeight="14580" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="benefits-drawbacks-pws" sheetId="1" r:id="rId1"/>
@@ -3256,8 +3256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>